<commit_message>
CRUD User And Template Admin LTE
</commit_message>
<xml_diff>
--- a/Hibah.xlsx
+++ b/Hibah.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCAD155-B273-4ACB-B9CA-68E446FF3916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="8655" yWindow="1200" windowWidth="8325" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I24" authorId="0" shapeId="0">
+    <comment ref="I24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N36" authorId="0" shapeId="0">
+    <comment ref="N36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t xml:space="preserve">tb_user </t>
   </si>
@@ -257,7 +258,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -336,7 +337,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Elbow Connector 2"/>
+        <xdr:cNvPr id="3" name="Elbow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -634,11 +641,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="J33" zoomScale="132" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Survei, Change bahasa and filter login
</commit_message>
<xml_diff>
--- a/Hibah.xlsx
+++ b/Hibah.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCAD155-B273-4ACB-B9CA-68E446FF3916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E6E55D-AC96-4DFC-85D7-6B1D42F41627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8655" yWindow="1200" windowWidth="8325" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="360" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -374,6 +374,206 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>423863</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>238090</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8399926-4C06-A6F4-B90F-77C3754F6FD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19854863" y="8524875"/>
+          <a:ext cx="4691027" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>288113</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>135713</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>125290</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>97613</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F3E5261-9687-42AE-EEF1-740E4E1F0B29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13623113" y="8327213"/>
+          <a:ext cx="4713977" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1714462</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>52350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>27639</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>14250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B12D498-7BDD-486B-8B40-CBC9B71819C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8077162" y="8243850"/>
+          <a:ext cx="4675877" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>116625</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>92812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>915827</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>54712</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D228E4D8-0B01-8896-33A8-40B1DF8989AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2593125" y="8284312"/>
+          <a:ext cx="4752077" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -644,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J33" zoomScale="132" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="D54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>